<commit_message>
Sorting for nicole wahahaha
</commit_message>
<xml_diff>
--- a/public/excel/PPEMNHTLYReport.xlsx
+++ b/public/excel/PPEMNHTLYReport.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="80">
   <si>
     <t>PPE MONTHLY REPORT</t>
   </si>
@@ -74,7 +74,7 @@
     <t>Ball Pen</t>
   </si>
   <si>
-    <t>02.500</t>
+    <t>02.510</t>
   </si>
   <si>
     <t>Supplies</t>
@@ -92,10 +92,7 @@
     <t>Notebook</t>
   </si>
   <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>Bernier, Jaylan</t>
+    <t>02.41</t>
   </si>
   <si>
     <t>00002</t>
@@ -107,7 +104,7 @@
     <t>Sticky Notes</t>
   </si>
   <si>
-    <t>01.50</t>
+    <t>01.51</t>
   </si>
   <si>
     <t>PRINT IMPRESS SUPPLIES &amp; SERVICES</t>
@@ -122,10 +119,7 @@
     <t>Monitor</t>
   </si>
   <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>Abshire, Eloisa</t>
+    <t>03.56</t>
   </si>
   <si>
     <t>DEL COMPUTER ENGRAVING SERVICES</t>
@@ -137,6 +131,9 @@
     <t>Mouse</t>
   </si>
   <si>
+    <t>02.11</t>
+  </si>
+  <si>
     <t>GIGATRON COMPUTER CENTER</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>System Unit</t>
   </si>
   <si>
-    <t>Bins, Jeff</t>
-  </si>
-  <si>
     <t>0008</t>
   </si>
   <si>
@@ -164,10 +158,13 @@
     <t xml:space="preserve">Endorsed To: </t>
   </si>
   <si>
-    <t>Jaclyn Iva Dietrich</t>
-  </si>
-  <si>
-    <t>Marielle Georgianna Kovacek</t>
+    <t>Boris Ida Stoltenberg</t>
+  </si>
+  <si>
+    <t>Cleta Meghan Koch</t>
+  </si>
+  <si>
+    <t>Colt Shaina Legros</t>
   </si>
   <si>
     <t>First Middle Last</t>
@@ -188,7 +185,7 @@
     <t>Water bottles</t>
   </si>
   <si>
-    <t>04</t>
+    <t>04.42</t>
   </si>
   <si>
     <t>AGUA BIYAYA WATER REFILLING STATION</t>
@@ -200,6 +197,9 @@
     <t>Water Dispenser</t>
   </si>
   <si>
+    <t>01.54</t>
+  </si>
+  <si>
     <t>2019-04-12</t>
   </si>
   <si>
@@ -209,10 +209,10 @@
     <t>Keyboard</t>
   </si>
   <si>
-    <t>19-2-0-0328-002</t>
-  </si>
-  <si>
-    <t>Anderson, Abel</t>
+    <t>01.57</t>
+  </si>
+  <si>
+    <t>2-19-03-29-001</t>
   </si>
   <si>
     <t>COMMUTER AUTO SUPPLY</t>
@@ -230,10 +230,10 @@
     <t>Ceiling fan</t>
   </si>
   <si>
-    <t>19-11-16-0425-000</t>
-  </si>
-  <si>
-    <t>Beahan, Vidal</t>
+    <t>03.21</t>
+  </si>
+  <si>
+    <t>11.16-19-04-11-001</t>
   </si>
   <si>
     <t>A.L.D. REFRIGERATION AIR CONDITIONING SERVICE</t>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>05.11</t>
+  </si>
+  <si>
+    <t>19-20-0-0101-105</t>
   </si>
   <si>
     <t>I</t>
@@ -811,7 +814,7 @@
   <cols>
     <col min="1" max="1" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="32.991943" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="4.570313" bestFit="true" customWidth="true" style="0"/>
@@ -947,7 +950,7 @@
         <v>10000</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K6" s="12">
         <v>0</v>
@@ -956,7 +959,7 @@
         <v>21</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -964,13 +967,13 @@
         <v>15</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>19</v>
@@ -992,10 +995,10 @@
         <v>0</v>
       </c>
       <c r="L7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="14" t="s">
         <v>30</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1003,13 +1006,13 @@
         <v>15</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>19</v>
@@ -1025,16 +1028,16 @@
         <v>144</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="K8" s="12">
         <v>0</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1042,13 +1045,13 @@
         <v>15</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>19</v>
@@ -1064,16 +1067,16 @@
         <v>121</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K9" s="12">
         <v>0</v>
       </c>
       <c r="L9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1081,13 +1084,13 @@
         <v>15</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>19</v>
@@ -1103,63 +1106,63 @@
         <v>144</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="K10" s="13">
         <v>0</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
         <v>48</v>
       </c>
-      <c r="C16" t="s">
+      <c r="G16" t="s">
         <v>49</v>
-      </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1201,10 +1204,10 @@
   <cols>
     <col min="1" max="1" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="32.991943" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="31.706543" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="18.709717" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="17.567139" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.996582" bestFit="true" customWidth="true" style="0"/>
@@ -1224,7 +1227,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1273,16 +1276,16 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>19</v>
@@ -1297,27 +1300,29 @@
       <c r="I5" s="10">
         <v>4761</v>
       </c>
-      <c r="J5" s="12"/>
+      <c r="J5" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="K5" s="12"/>
       <c r="L5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>54</v>
-      </c>
       <c r="C6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>19</v>
@@ -1332,10 +1337,12 @@
       <c r="I6" s="10">
         <v>9</v>
       </c>
-      <c r="J6" s="12"/>
+      <c r="J6" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="K6" s="12"/>
       <c r="L6" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M6" s="14">
         <v>5557</v>
@@ -1352,13 +1359,13 @@
         <v>62</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G7" s="11">
         <v>10</v>
@@ -1370,7 +1377,7 @@
         <v>100</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="K7" s="13">
         <v>0</v>
@@ -1384,49 +1391,49 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
         <v>48</v>
       </c>
-      <c r="C13" t="s">
+      <c r="G13" t="s">
         <v>49</v>
-      </c>
-      <c r="E13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1468,10 +1475,10 @@
   <cols>
     <col min="1" max="1" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="32.991943" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="31.706543" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="21.137695" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="22.280273" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.996582" bestFit="true" customWidth="true" style="0"/>
@@ -1549,13 +1556,13 @@
         <v>69</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G5" s="10">
         <v>5</v>
@@ -1567,7 +1574,7 @@
         <v>25</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="K5" s="12">
         <v>0</v>
@@ -1595,7 +1602,9 @@
       <c r="E6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="G6" s="11">
         <v>1</v>
       </c>
@@ -1606,13 +1615,13 @@
         <v>1</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M6" s="15">
         <v>456</v>
@@ -1620,49 +1629,49 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
         <v>48</v>
       </c>
-      <c r="C12" t="s">
+      <c r="G12" t="s">
         <v>49</v>
-      </c>
-      <c r="E12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Description per sort
</commit_message>
<xml_diff>
--- a/public/excel/PPEMNHTLYReport.xlsx
+++ b/public/excel/PPEMNHTLYReport.xlsx
@@ -18,7 +18,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
+  <si>
+    <t>All items by Joannie Abbey Bailey</t>
+  </si>
   <si>
     <t>PPE MONTHLY REPORT</t>
   </si>
@@ -164,13 +167,16 @@
     <t>Cleta Meghan Koch</t>
   </si>
   <si>
-    <t>Colt Shaina Legros</t>
-  </si>
-  <si>
-    <t>First Middle Last</t>
+    <t>Sherman Anika Bergnaum</t>
+  </si>
+  <si>
+    <t>Theresia Celine Willms</t>
   </si>
   <si>
     <t>City Accounting Department</t>
+  </si>
+  <si>
+    <t>City Assessor's Office</t>
   </si>
   <si>
     <t>April 01-April 30</t>
@@ -804,21 +810,21 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="L5" sqref="L5:M10"/>
+      <selection activeCell="L6" sqref="L6:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="39.990234" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="4.570313" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="26.993408" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="21.137695" bestFit="true" customWidth="true" style="0"/>
@@ -828,12 +834,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="D1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:13">
       <c r="D2" s="1" t="s">
@@ -843,337 +846,345 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="3" t="s">
+    <row r="3" spans="1:13">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="6" t="s">
+      <c r="M5" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="10">
-        <v>200</v>
-      </c>
-      <c r="H5" s="10">
-        <v>200</v>
-      </c>
-      <c r="I5" s="10">
-        <v>40000</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="12">
-        <v>0</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="10">
-        <v>100</v>
+        <v>200.0</v>
       </c>
       <c r="H6" s="10">
-        <v>100</v>
+        <v>200.0</v>
       </c>
       <c r="I6" s="10">
-        <v>10000</v>
+        <v>40000.0</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K6" s="12">
         <v>0</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="10">
-        <v>500</v>
+        <v>100.0</v>
       </c>
       <c r="H7" s="10">
-        <v>500</v>
+        <v>100.0</v>
       </c>
       <c r="I7" s="10">
-        <v>250000</v>
+        <v>10000.0</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K7" s="12">
         <v>0</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="10">
-        <v>12</v>
+        <v>500.0</v>
       </c>
       <c r="H8" s="10">
-        <v>12</v>
+        <v>500.0</v>
       </c>
       <c r="I8" s="10">
-        <v>144</v>
+        <v>250000.0</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K8" s="12">
         <v>0</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="10">
-        <v>11</v>
+        <v>12.0</v>
       </c>
       <c r="H9" s="10">
-        <v>11</v>
+        <v>12.0</v>
       </c>
       <c r="I9" s="10">
-        <v>121</v>
+        <v>144.0</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K9" s="12">
         <v>0</v>
       </c>
       <c r="L9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="E10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="10">
+        <v>11.0</v>
+      </c>
+      <c r="H10" s="10">
+        <v>11.0</v>
+      </c>
+      <c r="I10" s="10">
+        <v>121.0</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="M10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="11">
-        <v>12</v>
-      </c>
-      <c r="H10" s="11">
-        <v>12</v>
-      </c>
-      <c r="I10" s="11">
-        <v>144</v>
-      </c>
-      <c r="J10" s="13" t="s">
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="13">
+      <c r="F11" s="9"/>
+      <c r="G11" s="11">
+        <v>12.0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>12.0</v>
+      </c>
+      <c r="I11" s="11">
+        <v>144.0</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="13">
         <v>0</v>
       </c>
-      <c r="L10" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="2" t="s">
+      <c r="L11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" t="s">
-        <v>49</v>
-      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G17" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="D1:G1"/>
     <mergeCell ref="D2:G2"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:I14"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1194,21 +1205,21 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="L5" sqref="L5:M7"/>
+      <selection activeCell="L6" sqref="L6:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="39.990234" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="26.993408" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="21.137695" bestFit="true" customWidth="true" style="0"/>
@@ -1218,233 +1229,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="D1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:13">
       <c r="D2" s="1" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="3" spans="1:13">
+      <c r="D3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="10">
-        <v>69</v>
-      </c>
-      <c r="H5" s="10">
-        <v>69</v>
-      </c>
-      <c r="I5" s="10">
-        <v>4761</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>57</v>
+      <c r="M5" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="10">
-        <v>3</v>
+        <v>69.0</v>
       </c>
       <c r="H6" s="10">
-        <v>3</v>
+        <v>69.0</v>
       </c>
       <c r="I6" s="10">
-        <v>9</v>
+        <v>4761.0</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="M6" s="14">
+        <v>58</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="I7" s="10">
+        <v>9.0</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="12"/>
+      <c r="L7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" s="14">
         <v>5557</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="9" t="s">
+    <row r="8" spans="1:13">
+      <c r="A8" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="C8" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="11">
-        <v>10</v>
-      </c>
-      <c r="H7" s="11">
-        <v>10</v>
-      </c>
-      <c r="I7" s="11">
-        <v>100</v>
-      </c>
-      <c r="J7" s="13" t="s">
+      <c r="D8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="13">
+      <c r="F8" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="11">
+        <v>10.0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>10.0</v>
+      </c>
+      <c r="I8" s="11">
+        <v>100.0</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="13">
         <v>0</v>
       </c>
-      <c r="L7" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="M7" s="15">
+      <c r="L8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8" s="15">
         <v>1111</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
+    <row r="11" spans="1:13">
+      <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" t="s">
-        <v>49</v>
-      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G14" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="D1:G1"/>
     <mergeCell ref="D2:G2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:I11"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1465,21 +1481,21 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="L5" sqref="L5:M6"/>
+      <selection activeCell="L6" sqref="L6:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="39.990234" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="22.280273" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="26.993408" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="21.137695" bestFit="true" customWidth="true" style="0"/>
@@ -1489,200 +1505,205 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="D1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:13">
       <c r="D2" s="1" t="s">
-        <v>66</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="3" spans="1:13">
+      <c r="D3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="M5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="B6" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G5" s="10">
-        <v>5</v>
-      </c>
-      <c r="H5" s="10">
-        <v>5</v>
-      </c>
-      <c r="I5" s="10">
-        <v>25</v>
-      </c>
-      <c r="J5" s="12" t="s">
+      <c r="D6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="12">
+      <c r="F6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="H6" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="I6" s="10">
+        <v>25.0</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="12">
         <v>0</v>
       </c>
-      <c r="L5" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="M5" s="14">
+      <c r="L6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6" s="14">
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="9" t="s">
+    <row r="7" spans="1:13">
+      <c r="A7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="B7" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="9" t="s">
+      <c r="C7" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="G6" s="11">
-        <v>1</v>
-      </c>
-      <c r="H6" s="11">
-        <v>1</v>
-      </c>
-      <c r="I6" s="11">
-        <v>1</v>
-      </c>
-      <c r="J6" s="13" t="s">
+      <c r="D7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="L6" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="M6" s="15">
+      <c r="G7" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="I7" s="11">
+        <v>1.0</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="M7" s="15">
         <v>456</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
+    <row r="10" spans="1:13">
+      <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" t="s">
-        <v>49</v>
-      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="D1:G1"/>
     <mergeCell ref="D2:G2"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:I10"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>